<commit_message>
Added separate stories Excel file
</commit_message>
<xml_diff>
--- a/TPS Reports.xlsx
+++ b/TPS Reports.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\GitHub\quadratic-solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -86,13 +86,16 @@
     <t>Nate</t>
   </si>
   <si>
-    <t>Nate, Xavier, Ali</t>
-  </si>
-  <si>
     <t>5 min</t>
   </si>
   <si>
     <t>1 hr</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>20 min</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +585,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -599,7 +602,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -608,7 +611,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -620,7 +623,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -629,7 +632,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
@@ -653,13 +656,21 @@
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>